<commit_message>
Adding basic infrastructure + first analysis
</commit_message>
<xml_diff>
--- a/Project-Dataset.xlsx
+++ b/Project-Dataset.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f190256\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eqan Ahmad\Desktop\Starvation-Period-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4171B285-18A6-44FB-990A-9C37A3EE82E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Market Year</t>
   </si>
@@ -109,11 +119,14 @@
   <si>
     <t>Wheat Exports Growth Rate</t>
   </si>
+  <si>
+    <t>GDP Growth Rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -246,20 +259,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -274,9 +278,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -560,11 +561,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +584,7 @@
     <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,17 +657,20 @@
       <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1960</v>
       </c>
@@ -748,8 +752,11 @@
       <c r="AA2">
         <v>1.5087527882085687E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2" s="9">
+        <v>3.6538922501768024E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1961</v>
       </c>
@@ -801,13 +808,13 @@
       <c r="Q3">
         <v>-0.30167777997599798</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>0.11727672477811904</v>
       </c>
       <c r="S3">
         <v>-0.8555521911777616</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="8">
         <v>0.45045247518212433</v>
       </c>
       <c r="U3">
@@ -831,8 +838,11 @@
       <c r="AA3">
         <v>1.4076829373727031E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3">
+        <v>5.9900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1962</v>
       </c>
@@ -884,13 +894,13 @@
       <c r="Q4">
         <v>1.7327891148171695</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="9">
         <v>0.10828341866016003</v>
       </c>
       <c r="S4">
         <v>1.0282732267997952</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="8">
         <v>0.37326578499550245</v>
       </c>
       <c r="U4">
@@ -914,8 +924,11 @@
       <c r="AA4">
         <v>1.5832580951446316E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB4">
+        <v>4.48E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1963</v>
       </c>
@@ -967,13 +980,13 @@
       <c r="Q5">
         <v>-2.0553214597621623</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="9">
         <v>2.5601575551321108E-2</v>
       </c>
       <c r="S5">
         <v>-1.1480213174679066</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="8">
         <v>0.39720286248545111</v>
       </c>
       <c r="U5">
@@ -997,8 +1010,11 @@
       <c r="AA5">
         <v>1.41988762321195E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB5">
+        <v>8.6900000000000005E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1964</v>
       </c>
@@ -1050,13 +1066,13 @@
       <c r="Q6">
         <v>-0.64125538572029905</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="9">
         <v>0.11297631816879934</v>
       </c>
       <c r="S6">
         <v>1.3669045120968937</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="8">
         <v>0.45411089168240515</v>
       </c>
       <c r="U6">
@@ -1080,8 +1096,11 @@
       <c r="AA6">
         <v>1.2790154679523442E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB6">
+        <v>7.5700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1965</v>
       </c>
@@ -1133,13 +1152,13 @@
       <c r="Q7">
         <v>1.2476739947140407</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="9">
         <v>3.1179737574141515E-2</v>
       </c>
       <c r="S7">
         <v>1.7076360560876267</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="8">
         <v>0.39476734847226547</v>
       </c>
       <c r="U7">
@@ -1163,8 +1182,11 @@
       <c r="AA7">
         <v>1.3158755772171153E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>0.1042</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1966</v>
       </c>
@@ -1216,13 +1238,13 @@
       <c r="Q8">
         <v>1.3777649813367931</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="9">
         <v>0.12769271019917594</v>
       </c>
       <c r="S8">
         <v>-2.2100544998301301</v>
       </c>
-      <c r="T8" s="9">
+      <c r="T8" s="8">
         <v>0.44256927588025674</v>
       </c>
       <c r="U8">
@@ -1246,8 +1268,11 @@
       <c r="AA8">
         <v>1.5077588177123192E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB8">
+        <v>5.79E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1967</v>
       </c>
@@ -1299,13 +1324,13 @@
       <c r="Q9">
         <v>3.7279180981347078</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="9">
         <v>-0.12730731471975879</v>
       </c>
       <c r="S9">
         <v>2.918311433933614</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9" s="8">
         <v>0.50909843000877386</v>
       </c>
       <c r="U9">
@@ -1329,8 +1354,11 @@
       <c r="AA9">
         <v>1.5236760311593817E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB9">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1968</v>
       </c>
@@ -1382,13 +1410,13 @@
       <c r="Q10">
         <v>0.87711635428420709</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="9">
         <v>0.17244030397228757</v>
       </c>
       <c r="S10">
         <v>-0.53921902738624217</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="8">
         <v>0.60911860751453317</v>
       </c>
       <c r="U10">
@@ -1412,8 +1440,11 @@
       <c r="AA10">
         <v>1.3664255058130856E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB10">
+        <v>7.2300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1969</v>
       </c>
@@ -1465,13 +1496,13 @@
       <c r="Q11">
         <v>-1.5315320484137609</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="9">
         <v>0.15529257583180428</v>
       </c>
       <c r="S11">
         <v>3.4036013171825825</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="8">
         <v>0.56936905540168814</v>
       </c>
       <c r="U11">
@@ -1495,8 +1526,11 @@
       <c r="AA11">
         <v>1.4597972040209663E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB11">
+        <v>5.5100000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1970</v>
       </c>
@@ -1548,13 +1582,13 @@
       <c r="Q12">
         <v>-6.7455849457301542E-2</v>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="9">
         <v>0.1881078239184468</v>
       </c>
       <c r="S12">
         <v>-0.4833538030243435</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="8">
         <v>0.54211974779909455</v>
       </c>
       <c r="U12">
@@ -1578,8 +1612,11 @@
       <c r="AA12">
         <v>1.3827335442752251E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB12">
+        <v>0.1135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1971</v>
       </c>
@@ -1631,13 +1668,13 @@
       <c r="Q13">
         <v>3.08542560619069</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="9">
         <v>-7.4970473071504548E-2</v>
       </c>
       <c r="S13">
         <v>2.5588070996422214</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="8">
         <v>0.37195707578762394</v>
       </c>
       <c r="U13">
@@ -1661,8 +1698,11 @@
       <c r="AA13">
         <v>1.4449794269115792E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1972</v>
       </c>
@@ -1714,13 +1754,13 @@
       <c r="Q14">
         <v>1.0811287253727073</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="9">
         <v>-7.1171291739220632E-3</v>
       </c>
       <c r="S14">
         <v>0.23751833739024819</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="8">
         <v>0.33098449039871275</v>
       </c>
       <c r="U14">
@@ -1744,8 +1784,11 @@
       <c r="AA14">
         <v>1.5685880408053913E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB14">
+        <v>8.0999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1973</v>
       </c>
@@ -1797,13 +1840,13 @@
       <c r="Q15">
         <v>2.83821090292391</v>
       </c>
-      <c r="R15" s="10">
+      <c r="R15" s="9">
         <v>8.7229281852565108E-2</v>
       </c>
       <c r="S15">
         <v>-2.3432547218778002</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="8">
         <v>0.56906288761515467</v>
       </c>
       <c r="U15">
@@ -1827,8 +1870,11 @@
       <c r="AA15">
         <v>1.61396899596374E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB15">
+        <v>7.0599999999999996E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1974</v>
       </c>
@@ -1880,13 +1926,13 @@
       <c r="Q16">
         <v>0.45059592188896302</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="9">
         <v>-6.132492749199317E-2</v>
       </c>
       <c r="S16">
         <v>-2.4270281146497483</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="8">
         <v>0.44627050510664296</v>
       </c>
       <c r="U16">
@@ -1910,8 +1956,11 @@
       <c r="AA16">
         <v>1.5265710741067733E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB16">
+        <v>3.5400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1975</v>
       </c>
@@ -1963,13 +2012,13 @@
       <c r="Q17">
         <v>-0.34476330666134725</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="9">
         <v>-0.16344608198525667</v>
       </c>
       <c r="S17">
         <v>1.2158271576461881</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="8">
         <v>0.55189599750801666</v>
       </c>
       <c r="U17">
@@ -1993,8 +2042,11 @@
       <c r="AA17">
         <v>1.5193544220944965E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB17">
+        <v>4.2099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1976</v>
       </c>
@@ -2046,13 +2098,13 @@
       <c r="Q18">
         <v>-2.7039928273281717</v>
       </c>
-      <c r="R18" s="10">
+      <c r="R18" s="9">
         <v>0.10025857124693005</v>
       </c>
       <c r="S18">
         <v>1.4568720747677506</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="8">
         <v>0.535302121130518</v>
       </c>
       <c r="U18">
@@ -2076,8 +2128,11 @@
       <c r="AA18">
         <v>1.5561485735047438E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB18">
+        <v>5.16E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1977</v>
       </c>
@@ -2129,13 +2184,13 @@
       <c r="Q19">
         <v>-5.1794205957920294</v>
       </c>
-      <c r="R19" s="10">
+      <c r="R19" s="9">
         <v>-2.1455017826874069E-2</v>
       </c>
       <c r="S19">
         <v>2.8231528197541604</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19" s="8">
         <v>0.45292275822168382</v>
       </c>
       <c r="U19">
@@ -2159,8 +2214,11 @@
       <c r="AA19">
         <v>1.3487172343131326E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB19">
+        <v>3.95E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1978</v>
       </c>
@@ -2212,13 +2270,13 @@
       <c r="Q20">
         <v>0.84101758387060888</v>
       </c>
-      <c r="R20" s="10">
+      <c r="R20" s="9">
         <v>-9.8036717789944897E-2</v>
       </c>
       <c r="S20">
         <v>-2.9888389669277644</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="8">
         <v>0.37602299593641009</v>
       </c>
       <c r="U20">
@@ -2242,8 +2300,11 @@
       <c r="AA20">
         <v>1.5211168653708151E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB20">
+        <v>8.0500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1979</v>
       </c>
@@ -2295,13 +2356,13 @@
       <c r="Q21">
         <v>-2.8235331126039189</v>
       </c>
-      <c r="R21" s="10">
+      <c r="R21" s="9">
         <v>0.1562988120702673</v>
       </c>
       <c r="S21">
         <v>2.338166157310388</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="8">
         <v>0.47804731322888655</v>
       </c>
       <c r="U21">
@@ -2325,8 +2386,11 @@
       <c r="AA21">
         <v>1.3894426977506858E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB21">
+        <v>3.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1980</v>
       </c>
@@ -2378,13 +2442,13 @@
       <c r="Q22">
         <v>0.12972655731883895</v>
       </c>
-      <c r="R22" s="10">
+      <c r="R22" s="9">
         <v>9.5865308404970193E-2</v>
       </c>
       <c r="S22">
         <v>0.32489877184378424</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22" s="8">
         <v>0.4137873029103577</v>
       </c>
       <c r="U22">
@@ -2408,8 +2472,11 @@
       <c r="AA22">
         <v>1.3504272655937075E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB22">
+        <v>0.1022</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1981</v>
       </c>
@@ -2461,13 +2528,13 @@
       <c r="Q23">
         <v>0.74860847225409455</v>
       </c>
-      <c r="R23" s="10">
+      <c r="R23" s="9">
         <v>-5.7143449974591795E-2</v>
       </c>
       <c r="S23">
         <v>-0.37606576293282579</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23" s="8">
         <v>0.35321071167526796</v>
       </c>
       <c r="U23">
@@ -2491,8 +2558,11 @@
       <c r="AA23">
         <v>1.2798495225787241E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB23">
+        <v>7.9200000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1982</v>
       </c>
@@ -2544,13 +2614,13 @@
       <c r="Q24">
         <v>0.42376561821990122</v>
       </c>
-      <c r="R24" s="10">
+      <c r="R24" s="9">
         <v>5.8906414971014336E-2</v>
       </c>
       <c r="S24">
         <v>1.6456935665681756</v>
       </c>
-      <c r="T24" s="9">
+      <c r="T24" s="8">
         <v>0.43703380652540758</v>
       </c>
       <c r="U24">
@@ -2574,8 +2644,11 @@
       <c r="AA24">
         <v>1.4655713685737167E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB24">
+        <v>6.54E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1983</v>
       </c>
@@ -2627,13 +2700,13 @@
       <c r="Q25">
         <v>0.46843173439918617</v>
       </c>
-      <c r="R25" s="10">
+      <c r="R25" s="9">
         <v>-0.17147406024851813</v>
       </c>
       <c r="S25">
         <v>-2.1040515131132622</v>
       </c>
-      <c r="T25" s="9">
+      <c r="T25" s="8">
         <v>0.30701119163050616</v>
       </c>
       <c r="U25">
@@ -2657,8 +2730,11 @@
       <c r="AA25">
         <v>1.3757077018617926E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB25">
+        <v>6.7799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1984</v>
       </c>
@@ -2710,13 +2786,13 @@
       <c r="Q26">
         <v>1.0282739919381751</v>
       </c>
-      <c r="R26" s="10">
+      <c r="R26" s="9">
         <v>8.8429116866704197E-2</v>
       </c>
       <c r="S26">
         <v>-2.1959800352394212</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="8">
         <v>0.6473090702922456</v>
       </c>
       <c r="U26">
@@ -2740,8 +2816,11 @@
       <c r="AA26">
         <v>1.4673365740079689E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB26">
+        <v>5.0700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1985</v>
       </c>
@@ -2793,13 +2872,13 @@
       <c r="Q27">
         <v>0.9410917525807565</v>
       </c>
-      <c r="R27" s="10">
+      <c r="R27" s="9">
         <v>9.4637899507684253E-2</v>
       </c>
       <c r="S27">
         <v>1.6637297847959907</v>
       </c>
-      <c r="T27" s="9">
+      <c r="T27" s="8">
         <v>0.57988428065087383</v>
       </c>
       <c r="U27">
@@ -2823,8 +2902,11 @@
       <c r="AA27">
         <v>1.3940039505230418E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB27">
+        <v>7.5899999999999995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1986</v>
       </c>
@@ -2876,13 +2958,13 @@
       <c r="Q28">
         <v>-1.2269595265511906</v>
       </c>
-      <c r="R28" s="10">
+      <c r="R28" s="9">
         <v>-4.8817239597914668E-2</v>
       </c>
       <c r="S28">
         <v>2.3471308837767779</v>
       </c>
-      <c r="T28" s="9">
+      <c r="T28" s="8">
         <v>0.6225253108639679</v>
       </c>
       <c r="U28">
@@ -2906,8 +2988,11 @@
       <c r="AA28">
         <v>1.3823016384877231E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB28">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1987</v>
       </c>
@@ -2959,13 +3044,13 @@
       <c r="Q29">
         <v>-1.2061346981961338</v>
       </c>
-      <c r="R29" s="10">
+      <c r="R29" s="9">
         <v>-5.4256931874692362E-2</v>
       </c>
       <c r="S29">
         <v>1.1706703553023237</v>
       </c>
-      <c r="T29" s="9">
+      <c r="T29" s="8">
         <v>0.3956763734983989</v>
       </c>
       <c r="U29">
@@ -2989,8 +3074,11 @@
       <c r="AA29">
         <v>1.5181444215354983E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB29">
+        <v>6.4500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1988</v>
       </c>
@@ -3042,13 +3130,13 @@
       <c r="Q30">
         <v>0.92208336297087279</v>
       </c>
-      <c r="R30" s="10">
+      <c r="R30" s="9">
         <v>-9.7027175551032976E-2</v>
       </c>
       <c r="S30">
         <v>-0.34145420024811834</v>
       </c>
-      <c r="T30" s="9">
+      <c r="T30" s="8">
         <v>0.55323275262030502</v>
       </c>
       <c r="U30">
@@ -3072,8 +3160,11 @@
       <c r="AA30">
         <v>1.4677382756420929E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB30">
+        <v>7.6300000000000007E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1989</v>
       </c>
@@ -3125,13 +3216,13 @@
       <c r="Q31">
         <v>-0.80227177771396663</v>
       </c>
-      <c r="R31" s="10">
+      <c r="R31" s="9">
         <v>0.20490449788230175</v>
       </c>
       <c r="S31">
         <v>-0.23098384910371894</v>
       </c>
-      <c r="T31" s="9">
+      <c r="T31" s="8">
         <v>0.41080093117271321</v>
       </c>
       <c r="U31">
@@ -3155,8 +3246,11 @@
       <c r="AA31">
         <v>1.467819244185078E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB31">
+        <v>4.9599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1990</v>
       </c>
@@ -3208,13 +3302,13 @@
       <c r="Q32">
         <v>-0.9069370927754038</v>
       </c>
-      <c r="R32" s="10">
+      <c r="R32" s="9">
         <v>0.19907920487593631</v>
       </c>
       <c r="S32">
         <v>-2.3414762589635116</v>
       </c>
-      <c r="T32" s="9">
+      <c r="T32" s="8">
         <v>0.35094408461891841</v>
       </c>
       <c r="U32">
@@ -3238,8 +3332,11 @@
       <c r="AA32">
         <v>1.4404842947438556E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB32">
+        <v>4.4600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1991</v>
       </c>
@@ -3291,13 +3388,13 @@
       <c r="Q33">
         <v>-0.33023876027500865</v>
       </c>
-      <c r="R33" s="10">
+      <c r="R33" s="9">
         <v>-7.7864664030261752E-2</v>
       </c>
       <c r="S33">
         <v>-0.64422903177081403</v>
       </c>
-      <c r="T33" s="9">
+      <c r="T33" s="8">
         <v>0.57026182515573165</v>
       </c>
       <c r="U33">
@@ -3321,8 +3418,11 @@
       <c r="AA33">
         <v>5.8999999999999999E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB33">
+        <v>5.0599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1992</v>
       </c>
@@ -3374,13 +3474,13 @@
       <c r="Q34">
         <v>0.72531539232338682</v>
       </c>
-      <c r="R34" s="10">
+      <c r="R34" s="9">
         <v>-7.0582960188161473E-2</v>
       </c>
       <c r="S34">
         <v>-2.5193549325820963</v>
       </c>
-      <c r="T34" s="9">
+      <c r="T34" s="8">
         <v>0.45383460013494564</v>
       </c>
       <c r="U34">
@@ -3404,8 +3504,11 @@
       <c r="AA34">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB34">
+        <v>7.7100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1993</v>
       </c>
@@ -3457,13 +3560,13 @@
       <c r="Q35">
         <v>2.7970495270808735</v>
       </c>
-      <c r="R35" s="10">
+      <c r="R35" s="9">
         <v>-6.3649738356849825E-2</v>
       </c>
       <c r="S35">
         <v>2.5530881327359669</v>
       </c>
-      <c r="T35" s="9">
+      <c r="T35" s="8">
         <v>0.43786620534340032</v>
       </c>
       <c r="U35">
@@ -3487,8 +3590,11 @@
       <c r="AA35">
         <v>6.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB35">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1994</v>
       </c>
@@ -3540,13 +3646,13 @@
       <c r="Q36">
         <v>0.49016472662733745</v>
       </c>
-      <c r="R36" s="10">
+      <c r="R36" s="9">
         <v>5.6569933529785385E-2</v>
       </c>
       <c r="S36">
         <v>2.0527867860076041</v>
       </c>
-      <c r="T36" s="9">
+      <c r="T36" s="8">
         <v>0.46965759596527035</v>
       </c>
       <c r="U36">
@@ -3570,8 +3676,11 @@
       <c r="AA36">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB36">
+        <v>3.7400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1995</v>
       </c>
@@ -3623,13 +3732,13 @@
       <c r="Q37">
         <v>-0.16177238719144083</v>
       </c>
-      <c r="R37" s="10">
+      <c r="R37" s="9">
         <v>-0.12240318325515795</v>
       </c>
       <c r="S37">
         <v>5.9571892515804747E-2</v>
       </c>
-      <c r="T37" s="9">
+      <c r="T37" s="8">
         <v>0.52343433273126871</v>
       </c>
       <c r="U37">
@@ -3653,8 +3762,11 @@
       <c r="AA37">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB37">
+        <v>4.9599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1996</v>
       </c>
@@ -3706,13 +3818,13 @@
       <c r="Q38">
         <v>1.4469033124870014</v>
       </c>
-      <c r="R38" s="10">
+      <c r="R38" s="9">
         <v>-8.8235560491686571E-2</v>
       </c>
       <c r="S38">
         <v>5.9571892515804747E-2</v>
       </c>
-      <c r="T38" s="9">
+      <c r="T38" s="8">
         <v>0.63023972004324502</v>
       </c>
       <c r="U38">
@@ -3736,8 +3848,11 @@
       <c r="AA38">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB38">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1997</v>
       </c>
@@ -3789,13 +3904,13 @@
       <c r="Q39">
         <v>1.063756004302453</v>
       </c>
-      <c r="R39" s="10">
+      <c r="R39" s="9">
         <v>0.10321331534590322</v>
       </c>
       <c r="S39">
         <v>0.15340000000000001</v>
       </c>
-      <c r="T39" s="9">
+      <c r="T39" s="8">
         <v>0.15340000000000001</v>
       </c>
       <c r="U39">
@@ -3819,8 +3934,11 @@
       <c r="AA39">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB39">
+        <v>1.01E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1998</v>
       </c>
@@ -3872,13 +3990,13 @@
       <c r="Q40">
         <v>1.8438175491521158</v>
       </c>
-      <c r="R40" s="10">
+      <c r="R40" s="9">
         <v>2.4812780712380134E-2</v>
       </c>
       <c r="S40">
         <v>2.3E-2</v>
       </c>
-      <c r="T40" s="9">
+      <c r="T40" s="8">
         <v>2.4199999999999999E-2</v>
       </c>
       <c r="U40">
@@ -3902,8 +4020,11 @@
       <c r="AA40">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB40">
+        <v>2.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1999</v>
       </c>
@@ -3955,13 +4076,13 @@
       <c r="Q41">
         <v>5.3231504060193835E-2</v>
       </c>
-      <c r="R41" s="10">
+      <c r="R41" s="9">
         <v>0.14698660648298759</v>
       </c>
       <c r="S41">
         <v>2.4799999999999999E-2</v>
       </c>
-      <c r="T41" s="9">
+      <c r="T41" s="8">
         <v>2.3599999999999999E-2</v>
       </c>
       <c r="U41">
@@ -3985,8 +4106,11 @@
       <c r="AA41">
         <v>6.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB41">
+        <v>3.6600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2000</v>
       </c>
@@ -4038,13 +4162,13 @@
       <c r="Q42">
         <v>-1.3793556484317016</v>
       </c>
-      <c r="R42" s="10">
+      <c r="R42" s="9">
         <v>0.10450857372767308</v>
       </c>
       <c r="S42">
         <v>2.1899999999999999E-2</v>
       </c>
-      <c r="T42" s="9">
+      <c r="T42" s="8">
         <v>2.1899999999999999E-2</v>
       </c>
       <c r="U42">
@@ -4068,8 +4192,11 @@
       <c r="AA42">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB42">
+        <v>4.2599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2001</v>
       </c>
@@ -4121,13 +4248,13 @@
       <c r="Q43">
         <v>1.4822999392876861</v>
       </c>
-      <c r="R43" s="10">
+      <c r="R43" s="9">
         <v>-9.0299673508303716E-3</v>
       </c>
       <c r="S43">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="T43" s="9">
+      <c r="T43" s="8">
         <v>1.9199999999999998E-2</v>
       </c>
       <c r="U43">
@@ -4151,8 +4278,11 @@
       <c r="AA43">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB43">
+        <v>3.5499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2002</v>
       </c>
@@ -4204,13 +4334,13 @@
       <c r="Q44">
         <v>-0.67079140138653881</v>
       </c>
-      <c r="R44" s="10">
+      <c r="R44" s="9">
         <v>2.8268177148788268E-2</v>
       </c>
       <c r="S44">
         <v>2.4400000000000002E-2</v>
       </c>
-      <c r="T44" s="9">
+      <c r="T44" s="8">
         <v>2.4400000000000002E-2</v>
       </c>
       <c r="U44">
@@ -4234,8 +4364,11 @@
       <c r="AA44">
         <v>6.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB44">
+        <v>2.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2003</v>
       </c>
@@ -4287,13 +4420,13 @@
       <c r="Q45">
         <v>-0.29298757196945757</v>
       </c>
-      <c r="R45" s="10">
+      <c r="R45" s="9">
         <v>0.19874467400637483</v>
       </c>
       <c r="S45">
         <v>3.0300000000000001E-2</v>
       </c>
-      <c r="T45" s="9">
+      <c r="T45" s="8">
         <v>2.7E-2</v>
       </c>
       <c r="U45">
@@ -4317,8 +4450,11 @@
       <c r="AA45">
         <v>6.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB45">
+        <v>5.7799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2004</v>
       </c>
@@ -4370,13 +4506,13 @@
       <c r="Q46">
         <v>0</v>
       </c>
-      <c r="R46" s="10">
+      <c r="R46" s="9">
         <v>-0.10300389429972728</v>
       </c>
       <c r="S46">
         <v>2.7300000000000001E-2</v>
       </c>
-      <c r="T46" s="9">
+      <c r="T46" s="8">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="U46">
@@ -4400,8 +4536,11 @@
       <c r="AA46">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB46">
+        <v>7.5499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2005</v>
       </c>
@@ -4453,13 +4592,13 @@
       <c r="Q47">
         <v>0</v>
       </c>
-      <c r="R47" s="10">
+      <c r="R47" s="9">
         <v>0.15735452773667491</v>
       </c>
       <c r="S47">
         <v>2.5499999999999998E-2</v>
       </c>
-      <c r="T47" s="9">
+      <c r="T47" s="8">
         <v>2.87E-2</v>
       </c>
       <c r="U47">
@@ -4483,8 +4622,11 @@
       <c r="AA47">
         <v>6.1000000000000004E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB47">
+        <v>6.5199999999999994E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2006</v>
       </c>
@@ -4542,7 +4684,7 @@
       <c r="S48">
         <v>0.29480000000000001</v>
       </c>
-      <c r="T48" s="9">
+      <c r="T48" s="8">
         <v>0.29980000000000001</v>
       </c>
       <c r="U48">
@@ -4566,8 +4708,11 @@
       <c r="AA48">
         <v>5.7999999999999996E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB48">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2007</v>
       </c>
@@ -4625,7 +4770,7 @@
       <c r="S49">
         <v>3.3799999999999997E-2</v>
       </c>
-      <c r="T49" s="9">
+      <c r="T49" s="8">
         <v>2.9100000000000001E-2</v>
       </c>
       <c r="U49">
@@ -4649,8 +4794,11 @@
       <c r="AA49">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB49">
+        <v>4.8300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2008</v>
       </c>
@@ -4708,7 +4856,7 @@
       <c r="S50">
         <v>3.27E-2</v>
       </c>
-      <c r="T50" s="9">
+      <c r="T50" s="8">
         <v>2.46E-2</v>
       </c>
       <c r="U50">
@@ -4732,8 +4880,11 @@
       <c r="AA50">
         <v>4.1999999999999997E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB50">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2009</v>
       </c>
@@ -4791,7 +4942,7 @@
       <c r="S51">
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="T51" s="9">
+      <c r="T51" s="8">
         <v>3.0499999999999999E-2</v>
       </c>
       <c r="U51">
@@ -4815,8 +4966,11 @@
       <c r="AA51">
         <v>5.4000000000000003E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB51">
+        <v>2.8299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2010</v>
       </c>
@@ -4874,7 +5028,7 @@
       <c r="S52">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="T52" s="9">
+      <c r="T52" s="8">
         <v>3.0300000000000001E-2</v>
       </c>
       <c r="U52">
@@ -4898,8 +5052,11 @@
       <c r="AA52">
         <v>6.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB52">
+        <v>1.61E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2011</v>
       </c>
@@ -4957,7 +5114,7 @@
       <c r="S53">
         <v>3.4299999999999997E-2</v>
       </c>
-      <c r="T53" s="9">
+      <c r="T53" s="8">
         <v>3.56E-2</v>
       </c>
       <c r="U53">
@@ -4981,8 +5138,11 @@
       <c r="AA53">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB53">
+        <v>2.75E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2012</v>
       </c>
@@ -5040,7 +5200,7 @@
       <c r="S54">
         <v>3.32E-2</v>
       </c>
-      <c r="T54" s="9">
+      <c r="T54" s="8">
         <v>2.58E-2</v>
       </c>
       <c r="U54">
@@ -5064,8 +5224,11 @@
       <c r="AA54">
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB54">
+        <v>3.5099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2013</v>
       </c>
@@ -5123,7 +5286,7 @@
       <c r="S55">
         <v>2.7099999999999999E-2</v>
       </c>
-      <c r="T55" s="9">
+      <c r="T55" s="8">
         <v>2.4500000000000001E-2</v>
       </c>
       <c r="U55">
@@ -5147,8 +5310,11 @@
       <c r="AA55">
         <v>2.9499999999999998E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB55">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2014</v>
       </c>
@@ -5206,7 +5372,7 @@
       <c r="S56">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="T56" s="9">
+      <c r="T56" s="8">
         <v>3.27E-2</v>
       </c>
       <c r="U56">
@@ -5230,8 +5396,11 @@
       <c r="AA56">
         <v>1.83E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB56">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2015</v>
       </c>
@@ -5289,7 +5458,7 @@
       <c r="S57">
         <v>1.4800000000000001E-2</v>
       </c>
-      <c r="T57" s="9">
+      <c r="T57" s="8">
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="U57">
@@ -5313,8 +5482,11 @@
       <c r="AA57">
         <v>3.5700000000000003E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB57">
+        <v>4.7300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2016</v>
       </c>
@@ -5372,7 +5544,7 @@
       <c r="S58">
         <v>0.56107595947533606</v>
       </c>
-      <c r="T58" s="9">
+      <c r="T58" s="8">
         <v>0.36559590605890746</v>
       </c>
       <c r="U58">
@@ -5396,8 +5568,11 @@
       <c r="AA58">
         <v>3.78E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB58">
+        <v>5.5300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2017</v>
       </c>
@@ -5449,13 +5624,13 @@
       <c r="Q59">
         <v>-0.18066173483549747</v>
       </c>
-      <c r="R59" s="10">
+      <c r="R59" s="9">
         <v>-0.1735185234578695</v>
       </c>
       <c r="S59">
         <v>2.9616310411413824</v>
       </c>
-      <c r="T59" s="9">
+      <c r="T59" s="8">
         <v>0.51452129060881635</v>
       </c>
       <c r="U59">
@@ -5479,8 +5654,11 @@
       <c r="AA59">
         <v>3.9399999999999998E-2</v>
       </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB59">
+        <v>5.5500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2018</v>
       </c>
@@ -5532,13 +5710,13 @@
       <c r="Q60">
         <v>1.9923122279466932</v>
       </c>
-      <c r="R60" s="10">
+      <c r="R60" s="9">
         <v>-3.1291233603612328E-2</v>
       </c>
       <c r="S60">
         <v>0.81740352290213281</v>
       </c>
-      <c r="T60" s="9">
+      <c r="T60" s="8">
         <v>0.31104081964072794</v>
       </c>
       <c r="U60">
@@ -5562,8 +5740,11 @@
       <c r="AA60">
         <v>4.0800000000000003E-2</v>
       </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB60">
+        <v>5.8400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2019</v>
       </c>
@@ -5615,13 +5796,13 @@
       <c r="Q61">
         <v>3.4024388869183673</v>
       </c>
-      <c r="R61" s="10">
+      <c r="R61" s="9">
         <v>0.13486152502051027</v>
       </c>
       <c r="S61">
         <v>0.90512578743473138</v>
       </c>
-      <c r="T61" s="9">
+      <c r="T61" s="8">
         <v>0.46329452590341796</v>
       </c>
       <c r="U61">
@@ -5645,8 +5826,11 @@
       <c r="AA61">
         <v>3.9800000000000002E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB61">
+        <v>9.9000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2020</v>
       </c>
@@ -5698,13 +5882,13 @@
       <c r="Q62">
         <v>2.4210027567561663</v>
       </c>
-      <c r="R62" s="10">
+      <c r="R62" s="9">
         <v>0.16747477486155862</v>
       </c>
       <c r="S62">
         <v>-0.91129076188277425</v>
       </c>
-      <c r="T62" s="9">
+      <c r="T62" s="8">
         <v>0.51492067192349744</v>
       </c>
       <c r="U62">
@@ -5728,8 +5912,11 @@
       <c r="AA62">
         <v>4.65E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB62">
+        <v>5.3E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2021</v>
       </c>
@@ -5781,13 +5968,13 @@
       <c r="Q63">
         <v>-0.21039003528939326</v>
       </c>
-      <c r="R63" s="10">
+      <c r="R63" s="9">
         <v>0.18765492565146313</v>
       </c>
       <c r="S63">
         <v>1.0138597200312032</v>
       </c>
-      <c r="T63" s="9">
+      <c r="T63" s="8">
         <v>0.34269267609271381</v>
       </c>
       <c r="U63">
@@ -5811,8 +5998,11 @@
       <c r="AA63">
         <v>6.3E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AB63">
+        <v>4.1812677706704937E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>14</v>
       </c>
@@ -5821,7 +6011,7 @@
         <v>2.0322580645161245E-3</v>
       </c>
       <c r="C64" s="6">
-        <f t="shared" ref="C64:Z64" si="0">AVERAGE(C1:C63)</f>
+        <f t="shared" ref="C64:AB64" si="0">AVERAGE(C1:C63)</f>
         <v>-6.6612903225806456E-3</v>
       </c>
       <c r="D64" s="6">
@@ -5915,7 +6105,11 @@
         <v>0.18834230554529471</v>
       </c>
       <c r="AA64" s="6">
+        <f t="shared" si="0"/>
         <v>1.4311795996877872E-2</v>
+      </c>
+      <c r="AB64" s="6">
+        <v>5.0199219358201173E-2</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -5923,6 +6117,9 @@
     </row>
     <row r="68" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AA67:AD127">
+    <sortCondition ref="AA66:AA127"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding basic application with prediction ability
</commit_message>
<xml_diff>
--- a/Project-Dataset.xlsx
+++ b/Project-Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eqan Ahmad\Desktop\Starvation-Period-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305FCA29-FA50-4D3C-BAFF-4C195ED2C764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A197E6-A676-4C01-A702-C2BF07651058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -565,7 +565,7 @@
   <dimension ref="A1:AB68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="U67" sqref="U67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>